<commit_message>
excel file added '
</commit_message>
<xml_diff>
--- a/Akeem/Lessons in Excel v1.xlsx
+++ b/Akeem/Lessons in Excel v1.xlsx
@@ -5,17 +5,21 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\StudentsITeach\Akeem\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\StudentsWork-Lessons-\Akeem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08EB7EB5-4D2E-478A-8FE1-5748D2F970AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED26E781-03AF-4B09-B558-B5750FED6FBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{36FA73E8-9AB6-445D-991A-76F998077A32}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{36FA73E8-9AB6-445D-991A-76F998077A32}"/>
   </bookViews>
   <sheets>
     <sheet name="Data structures" sheetId="1" r:id="rId1"/>
+    <sheet name="forloop" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <pivotCaches>
+    <pivotCache cacheId="2" r:id="rId3"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
   <si>
     <t>Boy</t>
   </si>
@@ -105,6 +109,30 @@
   </si>
   <si>
     <t>names[0]</t>
+  </si>
+  <si>
+    <t>Ages</t>
+  </si>
+  <si>
+    <t>Age bracket</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>0-9</t>
+  </si>
+  <si>
+    <t>10-19</t>
+  </si>
+  <si>
+    <t>20+</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Count of Ages</t>
   </si>
 </sst>
 </file>
@@ -158,14 +186,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -181,6 +214,1095 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[Lessons in Excel v1.xlsx]forloop!PivotTable1</c:name>
+    <c:fmtId val="0"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>forloop!$G$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>forloop!$F$3:$F$6</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0-9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10-19</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20+</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>forloop!$G$3:$G$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-52CC-4371-8CDB-270E10BF09A5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+        <c14:dropZoneSeries val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{471602C9-92A7-D634-4608-5A6E0020118E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Windows User" refreshedDate="45082.750283912035" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="19" xr:uid="{F1C12C3C-0339-47A7-A585-1BB3AC7F8D4A}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:B20" sheet="forloop"/>
+  </cacheSource>
+  <cacheFields count="2">
+    <cacheField name="Ages" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="30"/>
+    </cacheField>
+    <cacheField name="Age bracket" numFmtId="0">
+      <sharedItems count="3">
+        <s v="10-19"/>
+        <s v="20+"/>
+        <s v="0-9"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="19">
+  <r>
+    <n v="16"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="28"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="6"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="29"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="5"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="12"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="24"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="14"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="27"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="24"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="26"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="7"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="15"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="20"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="5"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="30"/>
+    <x v="1"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E73BACF8-9BA5-4324-AEE4-212AF6B2D021}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="F2:G6" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="2">
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="2"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Ages" fld="0" subtotal="count" baseField="1" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="1">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -482,7 +1604,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31B1508E-44F2-41EF-9DE2-4D28F5CB7B02}">
   <dimension ref="A2:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8:D9"/>
     </sheetView>
   </sheetViews>
@@ -516,13 +1638,13 @@
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="4" t="s">
         <v>10</v>
       </c>
       <c r="K6" t="s">
@@ -533,57 +1655,57 @@
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="3"/>
+      <c r="B7" s="4"/>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="3"/>
+      <c r="E7" s="4"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="3"/>
+      <c r="B8" s="4"/>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="3"/>
+      <c r="E8" s="4"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="3"/>
+      <c r="B9" s="4"/>
       <c r="C9">
         <v>2</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="3"/>
+      <c r="E9" s="4"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="3"/>
+      <c r="B10" s="4"/>
       <c r="C10">
         <v>3</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="3"/>
+      <c r="E10" s="4"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="3"/>
-      <c r="E11" s="3"/>
+      <c r="B11" s="4"/>
+      <c r="E11" s="4"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
@@ -609,10 +1731,10 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D18" t="s">
@@ -650,4 +1772,253 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{359CE727-15D6-4F93-BD62-94E1A3B126B7}">
+  <dimension ref="A1:G20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>2</v>
+      </c>
+      <c r="B2" t="str">
+        <f ca="1">IF(A2&lt;10,"0-9",IF(A2&lt;20,"10-19","20+"))</f>
+        <v>0-9</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f t="shared" ref="A3:A20" ca="1" si="0">RANDBETWEEN(1,30)</f>
+        <v>17</v>
+      </c>
+      <c r="B3" t="str">
+        <f t="shared" ref="B3:B20" ca="1" si="1">IF(A3&lt;10,"0-9",IF(A3&lt;20,"10-19","20+"))</f>
+        <v>10-19</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B4" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>0-9</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f t="shared" ca="1" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B5" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>20+</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f t="shared" ca="1" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B6" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>20+</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="7">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f t="shared" ca="1" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B7" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>10-19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="B8" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>0-9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f t="shared" ca="1" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B9" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>20+</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f t="shared" ca="1" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B10" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>20+</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f t="shared" ca="1" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B11" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>20+</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f t="shared" ca="1" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B12" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>20+</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f t="shared" ca="1" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B13" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>20+</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f t="shared" ca="1" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B14" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>10-19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B15" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>0-9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f t="shared" ca="1" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B16" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>20+</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B17" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>0-9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f t="shared" ca="1" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B18" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>20+</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f t="shared" ca="1" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B19" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>20+</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <f t="shared" ca="1" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B20" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>20+</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>